<commit_message>
XLSX in other file
</commit_message>
<xml_diff>
--- a/v2 (extracted equations, json)/src/xlsx_results.xlsx
+++ b/v2 (extracted equations, json)/src/xlsx_results.xlsx
@@ -1547,16 +1547,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7593789384575185</c:v>
+                  <c:v>0.7574614069575467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8105877536414919</c:v>
+                  <c:v>0.8147544203081587</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7459386724386724</c:v>
+                  <c:v>0.7485225885225886</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6856241016674056</c:v>
+                  <c:v>0.6805608105281651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1603,16 +1603,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7645919103221627</c:v>
+                  <c:v>0.7583327329414622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8278307863938705</c:v>
+                  <c:v>0.8199258019701945</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7643956207628728</c:v>
+                  <c:v>0.7550469478528988</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6877218592173038</c:v>
+                  <c:v>0.6806665606933998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1659,16 +1659,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7614782472240014</c:v>
+                  <c:v>0.7545280383892298</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7977708175465186</c:v>
+                  <c:v>0.8021158331228424</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7357371255928866</c:v>
+                  <c:v>0.7390664436085137</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6913008106954914</c:v>
+                  <c:v>0.6797511301491156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1715,16 +1715,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7339801029356046</c:v>
+                  <c:v>0.7305966359581884</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.90439709101625</c:v>
+                  <c:v>0.9000995832280878</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.836179382147124</c:v>
+                  <c:v>0.8291025752920914</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5998964139204253</c:v>
+                  <c:v>0.5949825562425225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1771,16 +1771,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7274196041289688</c:v>
+                  <c:v>0.7295833569418475</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7708922286772754</c:v>
+                  <c:v>0.7688922286772754</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6975846529663985</c:v>
+                  <c:v>0.6972515417072379</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6482175017638971</c:v>
+                  <c:v>0.6529233841168383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1827,16 +1827,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7339009527299496</c:v>
+                  <c:v>0.7327469659732599</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8906782015660519</c:v>
+                  <c:v>0.8905948682327187</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8165983450753757</c:v>
+                  <c:v>0.8162939596879711</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6043580000055775</c:v>
+                  <c:v>0.6016913333389108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1883,16 +1883,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7237058324792378</c:v>
+                  <c:v>0.7273173180274553</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8737261303359434</c:v>
+                  <c:v>0.8909519870337628</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7958099208405394</c:v>
+                  <c:v>0.8151655488065874</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5921336601771985</c:v>
+                  <c:v>0.5895399477384469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2663,13 +2663,13 @@
         <v>27</v>
       </c>
       <c r="B3" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>0.8686868686868687</v>
+        <v>0.8682432432432432</v>
       </c>
       <c r="E3" s="2">
         <v>0.4482029598308668</v>
@@ -5828,16 +5828,16 @@
         <v>125</v>
       </c>
       <c r="D2" s="2">
-        <v>0.7593789384575185</v>
+        <v>0.7574614069575467</v>
       </c>
       <c r="E2" s="2">
-        <v>0.8105877536414919</v>
+        <v>0.8147544203081587</v>
       </c>
       <c r="F2" s="2">
-        <v>0.7459386724386724</v>
+        <v>0.7485225885225886</v>
       </c>
       <c r="G2" s="2">
-        <v>0.6856241016674056</v>
+        <v>0.6805608105281651</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5848,16 +5848,16 @@
         <v>125</v>
       </c>
       <c r="D3" s="2">
-        <v>0.7645919103221627</v>
+        <v>0.7583327329414622</v>
       </c>
       <c r="E3" s="2">
-        <v>0.8278307863938705</v>
+        <v>0.8199258019701945</v>
       </c>
       <c r="F3" s="2">
-        <v>0.7643956207628728</v>
+        <v>0.7550469478528988</v>
       </c>
       <c r="G3" s="2">
-        <v>0.6877218592173038</v>
+        <v>0.6806665606933998</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5868,16 +5868,16 @@
         <v>125</v>
       </c>
       <c r="D4" s="2">
-        <v>0.7614782472240014</v>
+        <v>0.7545280383892298</v>
       </c>
       <c r="E4" s="2">
-        <v>0.7977708175465186</v>
+        <v>0.8021158331228424</v>
       </c>
       <c r="F4" s="2">
-        <v>0.7357371255928866</v>
+        <v>0.7390664436085137</v>
       </c>
       <c r="G4" s="2">
-        <v>0.6913008106954914</v>
+        <v>0.6797511301491156</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5888,16 +5888,16 @@
         <v>125</v>
       </c>
       <c r="D5" s="2">
-        <v>0.7339801029356046</v>
+        <v>0.7305966359581884</v>
       </c>
       <c r="E5" s="2">
-        <v>0.90439709101625</v>
+        <v>0.9000995832280878</v>
       </c>
       <c r="F5" s="2">
-        <v>0.836179382147124</v>
+        <v>0.8291025752920914</v>
       </c>
       <c r="G5" s="2">
-        <v>0.5998964139204253</v>
+        <v>0.5949825562425225</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5908,16 +5908,16 @@
         <v>125</v>
       </c>
       <c r="D6" s="2">
-        <v>0.7274196041289688</v>
+        <v>0.7295833569418475</v>
       </c>
       <c r="E6" s="2">
-        <v>0.7708922286772754</v>
+        <v>0.7688922286772754</v>
       </c>
       <c r="F6" s="2">
-        <v>0.6975846529663985</v>
+        <v>0.6972515417072379</v>
       </c>
       <c r="G6" s="2">
-        <v>0.6482175017638971</v>
+        <v>0.6529233841168383</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5928,16 +5928,16 @@
         <v>125</v>
       </c>
       <c r="D7" s="2">
-        <v>0.7339009527299496</v>
+        <v>0.7327469659732599</v>
       </c>
       <c r="E7" s="2">
-        <v>0.8906782015660519</v>
+        <v>0.8905948682327187</v>
       </c>
       <c r="F7" s="2">
-        <v>0.8165983450753757</v>
+        <v>0.8162939596879711</v>
       </c>
       <c r="G7" s="2">
-        <v>0.6043580000055775</v>
+        <v>0.6016913333389108</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5948,16 +5948,16 @@
         <v>125</v>
       </c>
       <c r="D8" s="2">
-        <v>0.7237058324792378</v>
+        <v>0.7273173180274553</v>
       </c>
       <c r="E8" s="2">
-        <v>0.8737261303359434</v>
+        <v>0.8909519870337628</v>
       </c>
       <c r="F8" s="2">
-        <v>0.7958099208405394</v>
+        <v>0.8151655488065874</v>
       </c>
       <c r="G8" s="2">
-        <v>0.5921336601771985</v>
+        <v>0.5895399477384469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>